<commit_message>
Fix: Network error in UserManager, set default password to 123, add UI helper text
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Inventario" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -22,9 +22,6 @@
     <t>Mes</t>
   </si>
   <si>
-    <t>Año</t>
-  </si>
-  <si>
     <t>DIR</t>
   </si>
   <si>
@@ -61,15 +58,9 @@
     <t>CARGO</t>
   </si>
   <si>
-    <t>AÑO CARGO</t>
-  </si>
-  <si>
     <t>EXPTE</t>
   </si>
   <si>
-    <t>AÑO EXPTE</t>
-  </si>
-  <si>
     <t>CUIT</t>
   </si>
   <si>
@@ -262,12 +253,6 @@
     <t>Total Dif. NO conformadas - Accesorios</t>
   </si>
   <si>
-    <t>Recaudación Total</t>
-  </si>
-  <si>
-    <t>Recaudación Nominal</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -527,6 +512,21 @@
   </si>
   <si>
     <t>apoderado@contribuyente.com.ar</t>
+  </si>
+  <si>
+    <t>Anio</t>
+  </si>
+  <si>
+    <t>ANIO CARGO</t>
+  </si>
+  <si>
+    <t>ANIO EXPTE</t>
+  </si>
+  <si>
+    <t>Recaudacion Total</t>
+  </si>
+  <si>
+    <t>Recaudacion Nominal</t>
   </si>
 </sst>
 </file>
@@ -534,7 +534,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -1096,7 +1096,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1442,7 +1442,7 @@
   <dimension ref="A1:CF13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="CD3" sqref="CD3"/>
+      <selection activeCell="CA15" sqref="CA15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.1"/>
@@ -1766,250 +1766,250 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AO2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AP2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO2" s="1" t="s">
+      <c r="AR2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="AY2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="BA2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="BB2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ2" s="1" t="s">
+      <c r="BC2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BA2" s="1" t="s">
+      <c r="BD2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BB2" s="1" t="s">
+      <c r="BE2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BC2" s="1" t="s">
+      <c r="BF2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BD2" s="1" t="s">
+      <c r="BG2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BE2" s="1" t="s">
+      <c r="BH2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BF2" s="1" t="s">
+      <c r="BI2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BG2" s="1" t="s">
+      <c r="BJ2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BH2" s="1" t="s">
+      <c r="BK2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BI2" s="1" t="s">
+      <c r="BL2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ2" s="1" t="s">
+      <c r="BM2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BK2" s="1" t="s">
+      <c r="BN2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BL2" s="1" t="s">
+      <c r="BO2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BM2" s="1" t="s">
+      <c r="BP2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BN2" s="1" t="s">
+      <c r="BQ2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BO2" s="1" t="s">
+      <c r="BR2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BP2" s="1" t="s">
+      <c r="BS2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BQ2" s="1" t="s">
+      <c r="BT2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="BR2" s="1" t="s">
+      <c r="BU2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BS2" s="1" t="s">
+      <c r="BV2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BT2" s="1" t="s">
+      <c r="BW2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BU2" s="1" t="s">
+      <c r="BX2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BV2" s="1" t="s">
+      <c r="BY2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BW2" s="1" t="s">
+      <c r="BZ2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="BX2" s="1" t="s">
+      <c r="CA2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BY2" s="1" t="s">
+      <c r="CB2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="BZ2" s="1" t="s">
+      <c r="CC2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="CA2" s="1" t="s">
+      <c r="CD2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="CB2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="CC2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="CD2" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="CE2" s="1" t="s">
-        <v>82</v>
+        <v>169</v>
       </c>
       <c r="CF2" s="1" t="s">
-        <v>83</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:84">
@@ -2026,34 +2026,34 @@
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="O3" s="5">
         <v>33280</v>
@@ -2071,13 +2071,13 @@
         <v>30716472945</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="W3" s="6">
         <v>44945</v>
@@ -2086,45 +2086,45 @@
         <v>44938</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="Z3" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="AA3" s="5"/>
       <c r="AB3" s="5"/>
       <c r="AC3" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="AD3" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="AE3" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="AF3" s="7">
         <v>5.5E-2</v>
       </c>
       <c r="AG3" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="AH3" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="AI3" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="AJ3" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="AK3" s="6">
         <v>45660</v>
       </c>
       <c r="AL3" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="AM3" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="AN3" s="5"/>
       <c r="AO3" s="5"/>
@@ -2132,7 +2132,7 @@
       <c r="AQ3" s="5"/>
       <c r="AR3" s="6"/>
       <c r="AS3" s="10" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="AT3" s="5"/>
       <c r="AU3" s="5"/>
@@ -2204,34 +2204,34 @@
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F4" s="4">
         <v>1</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="O4" s="5">
         <v>35912</v>
@@ -2249,13 +2249,13 @@
         <v>30716472946</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="V4" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="W4" s="6">
         <v>45338</v>
@@ -2264,45 +2264,45 @@
         <v>45329</v>
       </c>
       <c r="Y4" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="Z4" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="AA4" s="5"/>
       <c r="AB4" s="5"/>
       <c r="AC4" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="AD4" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="AE4" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="AF4" s="7">
         <v>5.5E-2</v>
       </c>
       <c r="AG4" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="AH4" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="AI4" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="AJ4" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="AK4" s="6">
         <v>45768</v>
       </c>
       <c r="AL4" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="AM4" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="AN4" s="5"/>
       <c r="AO4" s="5"/>
@@ -2310,7 +2310,7 @@
       <c r="AQ4" s="5"/>
       <c r="AR4" s="6"/>
       <c r="AS4" s="10" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="AT4" s="5"/>
       <c r="AU4" s="5"/>
@@ -2374,34 +2374,34 @@
         <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F5" s="4">
         <v>1</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="M5" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="N5" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>133</v>
       </c>
       <c r="O5" s="5">
         <v>36665</v>
@@ -2419,13 +2419,13 @@
         <v>30716472947</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="U5" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="V5" s="5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="W5" s="6">
         <v>45457</v>
@@ -2434,42 +2434,42 @@
         <v>45455</v>
       </c>
       <c r="Y5" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="AA5" s="5"/>
       <c r="AB5" s="5"/>
       <c r="AC5" s="5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="AD5" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="AE5" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="AF5" s="7">
         <v>5.5E-2</v>
       </c>
       <c r="AG5" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="AH5" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="AI5" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="AJ5" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="AK5" s="6">
         <v>45972</v>
       </c>
       <c r="AL5" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="AM5" s="5"/>
       <c r="AN5" s="5"/>
@@ -2480,7 +2480,7 @@
         <v>45959</v>
       </c>
       <c r="AS5" s="10" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="AT5" s="5"/>
       <c r="AU5" s="5"/>
@@ -2546,34 +2546,34 @@
         <v>1</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F6" s="4">
         <v>1</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="O6" s="5">
         <v>37028</v>
@@ -2591,13 +2591,13 @@
         <v>30716472948</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="W6" s="6">
         <v>45506</v>
@@ -2606,7 +2606,7 @@
         <v>45505</v>
       </c>
       <c r="Y6" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="Z6" s="4">
         <v>2021</v>
@@ -2614,37 +2614,37 @@
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
       <c r="AC6" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="AD6" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="AE6" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="AF6" s="7">
         <v>5.5E-2</v>
       </c>
       <c r="AG6" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="AH6" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="AI6" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="AJ6" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="AK6" s="6">
         <v>45768</v>
       </c>
       <c r="AL6" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="AM6" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="AN6" s="5"/>
       <c r="AO6" s="5"/>
@@ -2652,7 +2652,7 @@
       <c r="AQ6" s="5"/>
       <c r="AR6" s="6"/>
       <c r="AS6" s="10" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="AT6" s="5"/>
       <c r="AU6" s="5"/>
@@ -2716,34 +2716,34 @@
         <v>1</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F7" s="4">
         <v>1</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="O7" s="5">
         <v>38786</v>
@@ -2761,13 +2761,13 @@
         <v>30716472949</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="V7" s="5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="W7" s="6">
         <v>45741</v>
@@ -2776,7 +2776,7 @@
         <v>45736</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="Z7" s="4">
         <v>2023</v>
@@ -2784,45 +2784,45 @@
       <c r="AA7" s="5"/>
       <c r="AB7" s="5"/>
       <c r="AC7" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="AD7" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="AE7" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="AF7" s="7">
         <v>0.08</v>
       </c>
       <c r="AG7" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH7" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI7" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AJ7" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="AH7" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="AI7" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="AJ7" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="AK7" s="6"/>
       <c r="AL7" s="5"/>
       <c r="AM7" s="5"/>
       <c r="AN7" s="5"/>
       <c r="AO7" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="AP7" s="5"/>
       <c r="AQ7" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="AR7" s="6">
         <v>45964</v>
       </c>
       <c r="AS7" s="10" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="AT7" s="5"/>
       <c r="AU7" s="5"/>
@@ -2878,34 +2878,34 @@
         <v>1</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="O8" s="5">
         <v>38774</v>
@@ -2923,13 +2923,13 @@
         <v>30716472950</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="W8" s="6">
         <v>45741</v>
@@ -2938,7 +2938,7 @@
         <v>45736</v>
       </c>
       <c r="Y8" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="Z8" s="4">
         <v>2023</v>
@@ -2946,45 +2946,45 @@
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
       <c r="AC8" s="5" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="AD8" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="AE8" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="AF8" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="AG8" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH8" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI8" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="AJ8" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="AH8" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="AI8" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="AJ8" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="AK8" s="6"/>
       <c r="AL8" s="5"/>
       <c r="AM8" s="5"/>
       <c r="AN8" s="5"/>
       <c r="AO8" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="AP8" s="5"/>
       <c r="AQ8" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="AR8" s="6">
         <v>45968</v>
       </c>
       <c r="AS8" s="10" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="AT8" s="5"/>
       <c r="AU8" s="5"/>
@@ -3040,34 +3040,34 @@
         <v>1</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="O9" s="5">
         <v>38779</v>
@@ -3085,13 +3085,13 @@
         <v>30716472951</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="V9" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="W9" s="6">
         <v>45741</v>
@@ -3100,7 +3100,7 @@
         <v>45736</v>
       </c>
       <c r="Y9" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="Z9" s="4">
         <v>2023</v>
@@ -3108,45 +3108,45 @@
       <c r="AA9" s="5"/>
       <c r="AB9" s="5"/>
       <c r="AC9" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="AD9" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="AE9" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="AF9" s="7">
         <v>0.08</v>
       </c>
       <c r="AG9" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH9" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI9" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ9" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="AH9" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="AI9" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="AJ9" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="AK9" s="6"/>
       <c r="AL9" s="5"/>
       <c r="AM9" s="5"/>
       <c r="AN9" s="5"/>
       <c r="AO9" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="AP9" s="5"/>
       <c r="AQ9" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="AR9" s="6">
         <v>45973</v>
       </c>
       <c r="AS9" s="10" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="AT9" s="5"/>
       <c r="AU9" s="5"/>
@@ -3202,34 +3202,34 @@
         <v>1</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="O10" s="5">
         <v>38780</v>
@@ -3247,13 +3247,13 @@
         <v>30716472952</v>
       </c>
       <c r="T10" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="V10" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="W10" s="6">
         <v>45741</v>
@@ -3262,7 +3262,7 @@
         <v>45736</v>
       </c>
       <c r="Y10" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="Z10" s="4">
         <v>2023</v>
@@ -3270,45 +3270,45 @@
       <c r="AA10" s="5"/>
       <c r="AB10" s="5"/>
       <c r="AC10" s="5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="AD10" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="AE10" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="AF10" s="7">
         <v>0.08</v>
       </c>
       <c r="AG10" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH10" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI10" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ10" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="AH10" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="AI10" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="AJ10" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="AK10" s="6"/>
       <c r="AL10" s="5"/>
       <c r="AM10" s="5"/>
       <c r="AN10" s="5"/>
       <c r="AO10" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="AP10" s="5"/>
       <c r="AQ10" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="AR10" s="6">
         <v>45972</v>
       </c>
       <c r="AS10" s="10" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="AT10" s="5"/>
       <c r="AU10" s="5"/>
@@ -3364,34 +3364,34 @@
         <v>1</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F11" s="4">
         <v>1</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="O11" s="5">
         <v>33280</v>
@@ -3409,13 +3409,13 @@
         <v>30716472953</v>
       </c>
       <c r="T11" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="V11" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="W11" s="6">
         <v>44945</v>
@@ -3424,45 +3424,45 @@
         <v>44938</v>
       </c>
       <c r="Y11" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="Z11" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="AA11" s="5"/>
       <c r="AB11" s="5"/>
       <c r="AC11" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="AD11" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="AE11" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="AF11" s="7">
         <v>5.5E-2</v>
       </c>
       <c r="AG11" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="AH11" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="AI11" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="AJ11" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="AK11" s="6">
         <v>45660</v>
       </c>
       <c r="AL11" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="AM11" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="AN11" s="5"/>
       <c r="AO11" s="5"/>
@@ -3470,7 +3470,7 @@
       <c r="AQ11" s="5"/>
       <c r="AR11" s="6"/>
       <c r="AS11" s="10" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="AT11" s="5"/>
       <c r="AU11" s="5"/>
@@ -3542,34 +3542,34 @@
         <v>1</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="O12" s="5">
         <v>35912</v>
@@ -3587,13 +3587,13 @@
         <v>30716472954</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="U12" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="W12" s="6">
         <v>45338</v>
@@ -3602,45 +3602,45 @@
         <v>45329</v>
       </c>
       <c r="Y12" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="Z12" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="AA12" s="5"/>
       <c r="AB12" s="5"/>
       <c r="AC12" s="5" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="AD12" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="AE12" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="AF12" s="7">
         <v>5.5E-2</v>
       </c>
       <c r="AG12" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="AH12" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="AI12" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="AJ12" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="AK12" s="6">
         <v>45768</v>
       </c>
       <c r="AL12" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="AM12" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="AN12" s="5"/>
       <c r="AO12" s="5"/>
@@ -3648,7 +3648,7 @@
       <c r="AQ12" s="5"/>
       <c r="AR12" s="6"/>
       <c r="AS12" s="10" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="AT12" s="5"/>
       <c r="AU12" s="5"/>
@@ -3712,34 +3712,34 @@
         <v>1</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F13" s="4">
         <v>1</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="O13" s="5">
         <v>36665</v>
@@ -3757,13 +3757,13 @@
         <v>30716472955</v>
       </c>
       <c r="T13" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="U13" s="5" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="V13" s="5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="W13" s="6">
         <v>45457</v>
@@ -3772,42 +3772,42 @@
         <v>45455</v>
       </c>
       <c r="Y13" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="Z13" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="AA13" s="5"/>
       <c r="AB13" s="5"/>
       <c r="AC13" s="5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="AD13" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="AE13" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="AF13" s="7">
         <v>5.5E-2</v>
       </c>
       <c r="AG13" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="AH13" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="AI13" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="AJ13" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="AK13" s="6">
         <v>45972</v>
       </c>
       <c r="AL13" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="AM13" s="5"/>
       <c r="AN13" s="5"/>
@@ -3818,7 +3818,7 @@
         <v>45959</v>
       </c>
       <c r="AS13" s="10" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="AT13" s="5"/>
       <c r="AU13" s="5"/>

</xml_diff>